<commit_message>
Mis a jour du CAD avec les nouvelles dimensions de chorde
</commit_message>
<xml_diff>
--- a/CAD/Glider_CAD_Dimensions.xlsx
+++ b/CAD/Glider_CAD_Dimensions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\MECH532\CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1056900-15D1-45F3-A793-ED140F932EB8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03ACEFB1-5CF6-4B61-8CBD-13A0AF441BC1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E0F262A-28DB-404C-B75B-3615829252C8}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{6E0F262A-28DB-404C-B75B-3615829252C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -669,13 +669,13 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="82.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -720,7 +720,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -756,7 +756,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2">
-        <v>0.1</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -817,7 +817,7 @@
       </c>
       <c r="B11" s="2">
         <f>B6*B4</f>
-        <v>0.18000000000000002</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>

</xml_diff>